<commit_message>
Update fixture XLSX for URL testing
</commit_message>
<xml_diff>
--- a/spec/fixtures/spreadsheets/Valid_Flickr_sheet.xlsx
+++ b/spec/fixtures/spreadsheets/Valid_Flickr_sheet.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3059" uniqueCount="1122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3059" uniqueCount="1127">
   <si>
     <t>image file name</t>
   </si>
@@ -3402,6 +3402,21 @@
   </si>
   <si>
     <t>problems</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/130616888@N02/35158503671</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/130616888@N02/35158508881</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/130616888@N02/34444669214</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/130616888@N02/34478571073</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/130616888@N02/34478572333</t>
   </si>
 </sst>
 </file>
@@ -3854,10 +3869,10 @@
   <dimension ref="A1:G1032228"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A39" sqref="A39:XFD39"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3868,19 +3883,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C1" s="14" t="s">
-        <v>192</v>
+        <v>1122</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>196</v>
+        <v>1123</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>204</v>
+        <v>1124</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>210</v>
+        <v>1125</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>219</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.2">
@@ -13420,14 +13435,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1"/>
-    <hyperlink ref="D1" r:id="rId2"/>
-    <hyperlink ref="E1" r:id="rId3"/>
-    <hyperlink ref="F1" r:id="rId4"/>
-    <hyperlink ref="G1" r:id="rId5"/>
+    <hyperlink ref="E1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">

</xml_diff>